<commit_message>
Add cert study workbook
</commit_message>
<xml_diff>
--- a/az305-od-fall-2022.xlsx
+++ b/az305-od-fall-2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\Desktop\az305\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214AEB88-737D-4DF7-86BA-B14BB646CF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCE9599-F7EB-4579-867C-050426DFD1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69B1149E-7896-42AC-94A1-994B0C641093}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" tabRatio="207" xr2:uid="{69B1149E-7896-42AC-94A1-994B0C641093}"/>
   </bookViews>
   <sheets>
     <sheet name="AZ-305" sheetId="1" r:id="rId1"/>
@@ -294,6 +294,7 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -583,19 +584,19 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>38099</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958413</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>352425</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+            <xdr:cNvPr id="1025" name="Check Box 1" descr="Reviewed" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
@@ -669,13 +670,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>304800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -687,7 +688,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -755,15 +756,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>19708</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>19708</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -773,7 +774,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -841,15 +842,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:colOff>962025</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -859,7 +860,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -927,15 +928,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -945,7 +946,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1013,15 +1014,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1031,7 +1032,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1099,15 +1100,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1117,7 +1118,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1185,15 +1186,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1203,7 +1204,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1271,15 +1272,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>63062</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>958412</xdr:colOff>
+          <xdr:colOff>962025</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1289,7 +1290,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1357,15 +1358,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1375,7 +1376,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1443,15 +1444,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>26277</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>216777</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1461,7 +1462,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1529,15 +1530,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1547,7 +1548,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1615,15 +1616,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:colOff>942975</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1633,7 +1634,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1701,15 +1702,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>32846</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>32846</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1719,7 +1720,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1787,15 +1788,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>19708</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>210208</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1805,7 +1806,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1873,15 +1874,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>367863</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>177363</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1891,7 +1892,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1959,15 +1960,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1977,7 +1978,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2045,15 +2046,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2063,7 +2064,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2131,15 +2132,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2149,7 +2150,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2217,15 +2218,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2235,7 +2236,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2303,15 +2304,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2321,7 +2322,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2389,15 +2390,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:colOff>942975</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2407,7 +2408,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2475,15 +2476,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2493,7 +2494,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2561,15 +2562,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>32846</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>223346</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2579,7 +2580,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2647,15 +2648,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2665,7 +2666,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2733,15 +2734,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2751,7 +2752,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2819,15 +2820,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2837,7 +2838,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2905,15 +2906,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2923,7 +2924,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2991,15 +2992,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3009,7 +3010,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3077,15 +3078,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>43355</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>170794</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>938705</xdr:colOff>
+          <xdr:colOff>942975</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>170794</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3095,7 +3096,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3163,15 +3164,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>177363</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>177363</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3181,7 +3182,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3249,15 +3250,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3267,7 +3268,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3335,15 +3336,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:colOff>933450</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3353,7 +3354,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3421,15 +3422,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>39415</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>229915</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3439,7 +3440,7 @@
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3507,15 +3508,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3525,7 +3526,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3593,15 +3594,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>19708</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>38</xdr:row>
-          <xdr:rowOff>19708</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3611,7 +3612,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3679,15 +3680,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>38</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3697,7 +3698,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3765,15 +3766,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3783,7 +3784,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3851,15 +3852,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>41</xdr:row>
-          <xdr:rowOff>6570</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3869,7 +3870,7 @@
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3937,15 +3938,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>41</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3955,7 +3956,7 @@
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4023,15 +4024,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4041,7 +4042,7 @@
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4109,15 +4110,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4127,7 +4128,7 @@
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4195,15 +4196,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>39415</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>229915</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4213,7 +4214,7 @@
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4281,15 +4282,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>45</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>46</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4299,7 +4300,7 @@
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4367,15 +4368,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>46</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4385,7 +4386,7 @@
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4453,15 +4454,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>46</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>183932</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4471,7 +4472,7 @@
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4539,15 +4540,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>48</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>49</xdr:row>
-          <xdr:rowOff>13139</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4557,7 +4558,7 @@
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4625,15 +4626,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>49</xdr:row>
-          <xdr:rowOff>26276</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>50</xdr:row>
-          <xdr:rowOff>26276</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4643,7 +4644,7 @@
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4711,15 +4712,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>50</xdr:row>
-          <xdr:rowOff>19707</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>19707</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4729,7 +4730,7 @@
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4797,15 +4798,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>19707</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>210207</xdr:rowOff>
+          <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4815,7 +4816,7 @@
                   <a14:compatExt spid="_x0000_s1074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4883,13 +4884,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>52</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>53</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4901,7 +4902,7 @@
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4969,15 +4970,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>52</xdr:row>
-          <xdr:rowOff>170793</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>53</xdr:row>
-          <xdr:rowOff>170793</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4987,7 +4988,7 @@
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5055,15 +5056,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>36786</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>53</xdr:row>
-          <xdr:rowOff>170793</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>932136</xdr:colOff>
+          <xdr:colOff>933450</xdr:colOff>
           <xdr:row>54</xdr:row>
-          <xdr:rowOff>170793</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5073,7 +5074,7 @@
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C4604A-92BE-3B37-2C2A-84F2F9827D2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5438,18 +5439,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C966253B-92C6-4C37-9A7B-F81AE44DB974}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="76.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" style="2" customWidth="1"/>
-    <col min="6" max="8" width="20.140625" customWidth="1"/>
+    <col min="6" max="8" width="20.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5505,7 +5507,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
@@ -5564,7 +5566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -5619,7 +5621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>33</v>
       </c>
@@ -5694,7 +5696,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>2</v>
       </c>
@@ -5822,14 +5824,15 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId3" name="Check Box 1">
+            <control shapeId="1025" r:id="rId4" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5851,7 +5854,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId4" name="Check Box 2">
+            <control shapeId="1026" r:id="rId5" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5873,7 +5876,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId5" name="Check Box 3">
+            <control shapeId="1027" r:id="rId6" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5895,7 +5898,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId6" name="Check Box 4">
+            <control shapeId="1028" r:id="rId7" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5907,8 +5910,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>962025</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5917,7 +5920,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId7" name="Check Box 5">
+            <control shapeId="1029" r:id="rId8" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5939,7 +5942,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId8" name="Check Box 6">
+            <control shapeId="1030" r:id="rId9" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5961,7 +5964,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId9" name="Check Box 7">
+            <control shapeId="1031" r:id="rId10" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -5983,7 +5986,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId10" name="Check Box 8">
+            <control shapeId="1032" r:id="rId11" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6005,7 +6008,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId11" name="Check Box 9">
+            <control shapeId="1033" r:id="rId12" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6027,7 +6030,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId12" name="Check Box 10">
+            <control shapeId="1034" r:id="rId13" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6049,7 +6052,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId13" name="Check Box 11">
+            <control shapeId="1035" r:id="rId14" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6071,7 +6074,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId14" name="Check Box 12">
+            <control shapeId="1036" r:id="rId15" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6093,7 +6096,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId15" name="Check Box 13">
+            <control shapeId="1037" r:id="rId16" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6105,8 +6108,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>942975</xdr:colOff>
-                    <xdr:row>15</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6115,7 +6118,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId16" name="Check Box 14">
+            <control shapeId="1038" r:id="rId17" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6137,7 +6140,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId17" name="Check Box 15">
+            <control shapeId="1039" r:id="rId18" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6159,7 +6162,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId18" name="Check Box 16">
+            <control shapeId="1040" r:id="rId19" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6181,7 +6184,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId19" name="Check Box 17">
+            <control shapeId="1041" r:id="rId20" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6203,7 +6206,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId20" name="Check Box 18">
+            <control shapeId="1042" r:id="rId21" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6225,7 +6228,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId21" name="Check Box 19">
+            <control shapeId="1043" r:id="rId22" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6247,7 +6250,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId22" name="Check Box 20">
+            <control shapeId="1044" r:id="rId23" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6269,7 +6272,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId23" name="Check Box 21">
+            <control shapeId="1045" r:id="rId24" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6291,7 +6294,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId24" name="Check Box 22">
+            <control shapeId="1046" r:id="rId25" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6303,8 +6306,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>942975</xdr:colOff>
-                    <xdr:row>23</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>371475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6313,7 +6316,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId25" name="Check Box 23">
+            <control shapeId="1047" r:id="rId26" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6335,7 +6338,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId26" name="Check Box 24">
+            <control shapeId="1048" r:id="rId27" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6357,7 +6360,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId27" name="Check Box 25">
+            <control shapeId="1049" r:id="rId28" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6379,7 +6382,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId28" name="Check Box 26">
+            <control shapeId="1050" r:id="rId29" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6401,7 +6404,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId29" name="Check Box 27">
+            <control shapeId="1051" r:id="rId30" name="Check Box 27">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6423,7 +6426,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1052" r:id="rId30" name="Check Box 28">
+            <control shapeId="1052" r:id="rId31" name="Check Box 28">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6445,7 +6448,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId31" name="Check Box 29">
+            <control shapeId="1053" r:id="rId32" name="Check Box 29">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6467,7 +6470,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId32" name="Check Box 30">
+            <control shapeId="1054" r:id="rId33" name="Check Box 30">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6489,7 +6492,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId33" name="Check Box 31">
+            <control shapeId="1055" r:id="rId34" name="Check Box 31">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6511,7 +6514,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId34" name="Check Box 32">
+            <control shapeId="1056" r:id="rId35" name="Check Box 32">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6533,7 +6536,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId35" name="Check Box 33">
+            <control shapeId="1057" r:id="rId36" name="Check Box 33">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6545,8 +6548,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>933450</xdr:colOff>
-                    <xdr:row>35</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:row>34</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6555,7 +6558,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1058" r:id="rId36" name="Check Box 34">
+            <control shapeId="1058" r:id="rId37" name="Check Box 34">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6577,7 +6580,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId37" name="Check Box 35">
+            <control shapeId="1059" r:id="rId38" name="Check Box 35">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6599,7 +6602,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId38" name="Check Box 36">
+            <control shapeId="1060" r:id="rId39" name="Check Box 36">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6621,7 +6624,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1061" r:id="rId39" name="Check Box 37">
+            <control shapeId="1061" r:id="rId40" name="Check Box 37">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6643,7 +6646,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId40" name="Check Box 38">
+            <control shapeId="1062" r:id="rId41" name="Check Box 38">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6665,7 +6668,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId41" name="Check Box 39">
+            <control shapeId="1063" r:id="rId42" name="Check Box 39">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6687,7 +6690,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1064" r:id="rId42" name="Check Box 40">
+            <control shapeId="1064" r:id="rId43" name="Check Box 40">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6709,7 +6712,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId43" name="Check Box 41">
+            <control shapeId="1065" r:id="rId44" name="Check Box 41">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6731,7 +6734,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId44" name="Check Box 42">
+            <control shapeId="1066" r:id="rId45" name="Check Box 42">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6753,7 +6756,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1067" r:id="rId45" name="Check Box 43">
+            <control shapeId="1067" r:id="rId46" name="Check Box 43">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6775,7 +6778,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1068" r:id="rId46" name="Check Box 44">
+            <control shapeId="1068" r:id="rId47" name="Check Box 44">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6797,7 +6800,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1069" r:id="rId47" name="Check Box 45">
+            <control shapeId="1069" r:id="rId48" name="Check Box 45">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6819,7 +6822,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1070" r:id="rId48" name="Check Box 46">
+            <control shapeId="1070" r:id="rId49" name="Check Box 46">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6841,7 +6844,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1071" r:id="rId49" name="Check Box 47">
+            <control shapeId="1071" r:id="rId50" name="Check Box 47">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6863,7 +6866,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1072" r:id="rId50" name="Check Box 48">
+            <control shapeId="1072" r:id="rId51" name="Check Box 48">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6885,7 +6888,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1073" r:id="rId51" name="Check Box 49">
+            <control shapeId="1073" r:id="rId52" name="Check Box 49">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6907,7 +6910,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1074" r:id="rId52" name="Check Box 50">
+            <control shapeId="1074" r:id="rId53" name="Check Box 50">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6929,7 +6932,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1075" r:id="rId53" name="Check Box 51">
+            <control shapeId="1075" r:id="rId54" name="Check Box 51">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6951,7 +6954,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1076" r:id="rId54" name="Check Box 52">
+            <control shapeId="1076" r:id="rId55" name="Check Box 52">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>
@@ -6973,7 +6976,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1077" r:id="rId55" name="Check Box 53">
+            <control shapeId="1077" r:id="rId56" name="Check Box 53">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Reviewed">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>